<commit_message>
Update results XLS data and generate images.
</commit_message>
<xml_diff>
--- a/.results/limits/Data_GT650M.xlsx
+++ b/.results/limits/Data_GT650M.xlsx
@@ -359,10 +359,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -757,20 +757,39 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="53334528"/>
-        <c:axId val="135238144"/>
+        <c:axId val="112571904"/>
+        <c:axId val="86598784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="53334528"/>
+        <c:axId val="112571904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Data variant</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135238144"/>
+        <c:crossAx val="86598784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -778,18 +797,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135238144"/>
+        <c:axId val="86598784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Speedup [1]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53334528"/>
+        <c:crossAx val="112571904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -818,10 +856,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -1216,20 +1254,39 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="59075584"/>
-        <c:axId val="131392064"/>
+        <c:axId val="112573952"/>
+        <c:axId val="86601088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59075584"/>
+        <c:axId val="112573952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Data variant</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131392064"/>
+        <c:crossAx val="86601088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1237,18 +1294,42 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="131392064"/>
+        <c:axId val="86601088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Speedup </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>[1]</a:t>
+                </a:r>
+                <a:endParaRPr lang="cs-CZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59075584"/>
+        <c:crossAx val="112573952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1277,10 +1358,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -1438,11 +1519,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="100407488"/>
-        <c:axId val="100406912"/>
+        <c:axId val="86603392"/>
+        <c:axId val="86603968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100407488"/>
+        <c:axId val="86603392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1458,16 +1539,9 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="cs-CZ" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>Subset count [1]</a:t>
+                  <a:rPr lang="cs-CZ"/>
+                  <a:t>Subset count [1] </a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="cs-CZ" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
-                  <a:t> </a:t>
-                </a:r>
-                <a:endParaRPr lang="cs-CZ"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1478,12 +1552,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100406912"/>
+        <c:crossAx val="86603968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100406912"/>
+        <c:axId val="86603968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1514,7 +1588,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100407488"/>
+        <c:crossAx val="86603392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1926,7 +2000,7 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>